<commit_message>
run and some fix
</commit_message>
<xml_diff>
--- a/trained_models/cup2023/results_test_optuna_nn.xlsx
+++ b/trained_models/cup2023/results_test_optuna_nn.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.218418657563112</v>
+        <v>2.161735577932661</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9916505076009531</v>
+        <v>0.9928586087949914</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.550357293749737</v>
+        <v>1.48309608044758</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.403607738283007</v>
+        <v>2.199573983838975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>